<commit_message>
added more pa statuses
</commit_message>
<xml_diff>
--- a/data/input/participation_agreement_status.xlsx
+++ b/data/input/participation_agreement_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobertSurridge\Projects\reach_pa_upload\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EDE03C-34AA-4B5F-A1BD-C5C771F1F7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECD714D-8DE1-4A47-9474-B13BC1522AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="222">
   <si>
     <t>060160925022002</t>
   </si>
@@ -760,6 +760,27 @@
   </si>
   <si>
     <t>280000000009301</t>
+  </si>
+  <si>
+    <t>560990860052007</t>
+  </si>
+  <si>
+    <t>390550610253004</t>
+  </si>
+  <si>
+    <t>350590050262001</t>
+  </si>
+  <si>
+    <t>480723100160001</t>
+  </si>
+  <si>
+    <t>350500020262002</t>
+  </si>
+  <si>
+    <t>480721500251015</t>
+  </si>
+  <si>
+    <t>09010004X100000</t>
   </si>
 </sst>
 </file>
@@ -1071,11 +1092,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B223"/>
+  <dimension ref="A1:B230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2861,12 +2882,68 @@
         <v>45669.609236111108</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B223" s="9">
         <v>45671.485821759263</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B224" s="5">
+        <v>45680.349710648145</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B225" s="5">
+        <v>45681.353032407409</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B226" s="9">
+        <v>45684.438819444447</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B227" s="5">
+        <v>45685.536886574075</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B228" s="5">
+        <v>45685.58011574074</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B229" s="5">
+        <v>45687.35255787037</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B230" s="9">
+        <v>45687.389756944445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>